<commit_message>
Add Violations_Summary sheet with violation counts using COUNTIF
</commit_message>
<xml_diff>
--- a/user_access_inventory.xlsx
+++ b/user_access_inventory.xlsx
@@ -1,20 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaive\IT-Access-Audit\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E196F7C0-15E5-4B94-BC89-FA4648B4E3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="5180" yWindow="3900" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Violations_Summary" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="57">
   <si>
     <t>Username</t>
   </si>
@@ -164,16 +184,37 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>A (Violation Type)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	B (Count)</t>
+  </si>
+  <si>
+    <t>MFA</t>
+  </si>
+  <si>
+    <t>Password Age &gt; 90 Days</t>
+  </si>
+  <si>
+    <t>Inactive &gt; 60 Days</t>
+  </si>
+  <si>
+    <t>Terminated but Active</t>
+  </si>
+  <si>
+    <t>Admin Review Overdue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +229,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -225,25 +271,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -281,7 +344,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -315,6 +378,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -349,9 +413,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -524,12 +589,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
@@ -1262,4 +1327,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F907E9-5E6C-433F-9755-5B4BB33FD4E0}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="43.5">
+      <c r="A1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="5">
+        <f>COUNTIF(Sheet1!K2:K31, 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="43.5">
+      <c r="A3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="5">
+        <f>COUNTIF(Sheet1!L2:L31, 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="29">
+      <c r="A4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="5">
+        <f>COUNTIF(Sheet1!M2:M31, 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="43.5">
+      <c r="A5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="5">
+        <f>COUNTIF(Sheet1!N2:N31, 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="43.5">
+      <c r="A6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="5">
+        <f>COUNTIF(Sheet1!O2:O31, 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Total Risk Score column to Sheet1 using SUM of violation flags
</commit_message>
<xml_diff>
--- a/user_access_inventory.xlsx
+++ b/user_access_inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaive\IT-Access-Audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E196F7C0-15E5-4B94-BC89-FA4648B4E3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97D0A0B-BF82-4352-81A1-3DF4F2149AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3900" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5180" yWindow="3900" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="58">
   <si>
     <t>Username</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Admin Review Overdue</t>
+  </si>
+  <si>
+    <t>Total Risk Score</t>
   </si>
 </sst>
 </file>
@@ -244,7 +247,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -267,11 +270,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -285,6 +299,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,13 +607,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,8 +640,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -644,8 +666,12 @@
       <c r="H2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <f>SUM(K2:O2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -668,7 +694,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -691,7 +717,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -714,7 +740,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -737,7 +763,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -760,7 +786,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -783,7 +809,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -806,7 +832,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -829,7 +855,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -852,7 +878,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -878,7 +904,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -901,7 +927,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -924,7 +950,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -950,7 +976,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1333,7 +1359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F907E9-5E6C-433F-9755-5B4BB33FD4E0}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add Risk Level classification column to user_access_inventory.xlsx
</commit_message>
<xml_diff>
--- a/user_access_inventory.xlsx
+++ b/user_access_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaive\IT-Access-Audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97D0A0B-BF82-4352-81A1-3DF4F2149AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899720D5-5FE8-4C64-8254-40B99FF28095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3900" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="59">
   <si>
     <t>Username</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Total Risk Score</t>
+  </si>
+  <si>
+    <t>Risk Level</t>
   </si>
 </sst>
 </file>
@@ -285,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -299,6 +302,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -607,7 +613,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
@@ -615,7 +621,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -643,8 +649,11 @@
       <c r="I1" s="6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -670,8 +679,12 @@
         <f>SUM(K2:O2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" t="str">
+        <f>IF(P2=0, "Low", IF(P2&lt;=2, "Medium", "High"))</f>
+        <v>Low</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -694,7 +707,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -717,7 +730,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -740,7 +753,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -763,7 +776,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -786,7 +799,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -809,7 +822,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -832,7 +845,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -855,7 +868,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -878,7 +891,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -904,7 +917,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -927,7 +940,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -950,7 +963,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -976,7 +989,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>22</v>
       </c>

</xml_diff>